<commit_message>
ud bulk order files
</commit_message>
<xml_diff>
--- a/frontend/public/media/kemlabels-bulk-order-template.xlsx
+++ b/frontend/public/media/kemlabels-bulk-order-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_shippinglabels\ShippingProject\frontend\public\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elber\Documents\GitHub\ShippingProject\frontend\public\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6102C59E-309F-4109-A525-839833D17205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271BA63D-2457-4AAA-B30D-32BCAFD69A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18300" yWindow="6330" windowWidth="10890" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="1950" windowWidth="24795" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kemlabels-bulk-order-template" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+  <si>
+    <t>USPS</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
   <si>
     <t>FromCountry</t>
   </si>
@@ -47,12 +53,12 @@
     <t>FromName</t>
   </si>
   <si>
-    <t>FromCompany</t>
-  </si>
-  <si>
     <t>FromStreet1</t>
   </si>
   <si>
+    <t>FromStreet2 (Optional)</t>
+  </si>
+  <si>
     <t>FromCity</t>
   </si>
   <si>
@@ -68,12 +74,15 @@
     <t>ToName</t>
   </si>
   <si>
-    <t>ToCompany</t>
+    <t>ToPhone (Optional)</t>
   </si>
   <si>
     <t>ToStreet1</t>
   </si>
   <si>
+    <t>ToStreet2 (Optional)</t>
+  </si>
+  <si>
     <t>ToCity</t>
   </si>
   <si>
@@ -95,74 +104,62 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>FromPhone (optional)</t>
-  </si>
-  <si>
-    <t>FromStreet2 (Optional)</t>
-  </si>
-  <si>
-    <t>ToPhone (Optional)</t>
-  </si>
-  <si>
-    <t>ToStreet2 (Optional)</t>
-  </si>
-  <si>
     <t>Description (Optional)</t>
   </si>
   <si>
-    <t>Description2 (Optional)</t>
-  </si>
-  <si>
-    <t>USPS</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>UPS Express Early</t>
-  </si>
-  <si>
-    <t>UPS Express</t>
-  </si>
-  <si>
-    <t>UPS Express Saver</t>
-  </si>
-  <si>
-    <t>UPS Expedited</t>
-  </si>
-  <si>
-    <t>UPS Next Day Air Early</t>
-  </si>
-  <si>
-    <t>UPS Next Day Air</t>
-  </si>
-  <si>
-    <t>UPS 2nd Day Air</t>
-  </si>
-  <si>
-    <t>UPS 3 Day Select</t>
-  </si>
-  <si>
-    <t>UPS Ground</t>
-  </si>
-  <si>
-    <t>UPS Standard</t>
-  </si>
-  <si>
-    <t>USPS Ground Advantage</t>
-  </si>
-  <si>
-    <t>USPS Express</t>
-  </si>
-  <si>
-    <t>USPS Priority</t>
+    <t>ReferenceNumber</t>
+  </si>
+  <si>
+    <t>ReferenceNumber (Optional)</t>
+  </si>
+  <si>
+    <t>FromPhone (Optional)</t>
+  </si>
+  <si>
+    <t>Ground Advantage: 1-5 days</t>
+  </si>
+  <si>
+    <t>Priority: 1-3 days</t>
+  </si>
+  <si>
+    <t>Express: 1-2 days</t>
+  </si>
+  <si>
+    <t>Express Early: 1 day</t>
+  </si>
+  <si>
+    <t>Next Day Air Early: 1 day</t>
+  </si>
+  <si>
+    <t>Next Day Air: 1 day</t>
+  </si>
+  <si>
+    <t>2nd Day Air: 2 days</t>
+  </si>
+  <si>
+    <t>3 Day Select: 3 days</t>
+  </si>
+  <si>
+    <t>Ground: Min 3 days</t>
+  </si>
+  <si>
+    <t>Express: 1 day</t>
+  </si>
+  <si>
+    <t>Express Saver: 1 day</t>
+  </si>
+  <si>
+    <t>Expedited: 2 days</t>
+  </si>
+  <si>
+    <t>Standard: Flexible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +290,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -639,10 +642,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1019,131 +1025,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X2"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D6" activeCellId="1" sqref="D9 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5703125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7" style="1" customWidth="1"/>
+    <col min="20" max="20" width="7.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="21" style="1" customWidth="1"/>
+    <col min="23" max="23" width="27.7109375" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="S2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="T2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="U2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" t="s">
-        <v>16</v>
-      </c>
-      <c r="V2" t="s">
-        <v>17</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="V2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X2" t="s">
+      <c r="W2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="257" yWindow="264" count="4">
+  <phoneticPr fontId="18" type="noConversion"/>
+  <dataValidations xWindow="257" yWindow="264" count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Courier" prompt="Please select a courier" sqref="A1" xr:uid="{BC05BADB-F766-4E79-BCB6-8075CB7A0E72}">
       <formula1>"USPS, UPSUSA, UPSCA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{650D54CB-BF92-4196-AE09-D884D4DE9B58}">
-      <formula1>$A$6:$A$8</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Select YES or NO" promptTitle="Signature" prompt="Please select 'Yes' for signature." sqref="C1" xr:uid="{936E74DA-DDE8-40E6-8088-3041A2A45579}">
       <formula1>"YES, NO"</formula1>
@@ -1153,15 +1156,17 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C24CA1E-6A53-43D2-BC51-178472C3C247}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,51 +1178,51 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>